<commit_message>
Ch 5 and images
</commit_message>
<xml_diff>
--- a/graphmaking/overview graphs.xlsx
+++ b/graphmaking/overview graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arjan\Desktop\thesis\thesis-report\graphmaking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF059A63-CA88-4446-9C28-12CA1F8DCD9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E6A3F7-46C2-400A-9844-C90673A5B9F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2250" windowWidth="29040" windowHeight="15840" xr2:uid="{BA488DB3-6E91-463F-BA31-737BC2C97C80}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="123">
   <si>
     <t>Chapter</t>
   </si>
@@ -400,6 +400,9 @@
   </si>
   <si>
     <t>vergelijking van overfitting voor single orbit vs circular vs free</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -754,7 +757,7 @@
   <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1319,6 +1322,9 @@
       <c r="C40" t="s">
         <v>82</v>
       </c>
+      <c r="D40" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
@@ -1329,6 +1335,9 @@
       </c>
       <c r="C41" t="s">
         <v>83</v>
+      </c>
+      <c r="D41" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>